<commit_message>
import benef under production screen - phase 1
</commit_message>
<xml_diff>
--- a/ProjectX/wwwroot/Samplefile/beneficiaries.xlsx
+++ b/ProjectX/wwwroot/Samplefile/beneficiaries.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rashad.zeineddine\source\repos\mussa87\ProjectN\ProjectX\wwwroot\Samplefile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EBA048-51F3-483E-A229-B0E3F56203DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DCCF9B-DDAF-4E25-935C-55EBFCB8151D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="manual" sheetId="1" r:id="rId1"/>
+    <sheet name="Beneficiaries" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -63,7 +63,7 @@
     <t>Lname</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>